<commit_message>
Update DateBase/orders/Fresh bloom Flowers_2024-11-12.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/Fresh bloom Flowers_2024-11-12.xlsx
+++ b/DateBase/orders/Fresh bloom Flowers_2024-11-12.xlsx
@@ -445,6 +445,9 @@
       <c r="C2" t="str">
         <v>316_尤加利叶大叶_Eucalyptus Cinerea_undefined_1bunch</v>
       </c>
+      <c r="F2" t="str">
+        <v>2</v>
+      </c>
     </row>
     <row r="3">
       <c r="C3" t="str">
@@ -510,8 +513,8 @@
       <c r="F2" t="str">
         <v>0.00</v>
       </c>
-      <c r="G2">
-        <v>0</v>
+      <c r="G2" t="str">
+        <v>020</v>
       </c>
     </row>
   </sheetData>

</xml_diff>